<commit_message>
populated data2.xlsx and data3.xlsx
</commit_message>
<xml_diff>
--- a/data1.xlsx
+++ b/data1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\itapp\PycharmProjects\WLalgorithm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA6F0993-C357-41A9-AA2B-4CD5EAFF4D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E918FDE-C544-47B5-BA1A-C47A39436E52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1842,13 +1842,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>14343</xdr:colOff>
+      <xdr:colOff>14344</xdr:colOff>
       <xdr:row>151</xdr:row>
       <xdr:rowOff>129316</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>519952</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>600636</xdr:colOff>
       <xdr:row>175</xdr:row>
       <xdr:rowOff>8965</xdr:rowOff>
     </xdr:to>
@@ -2166,7 +2166,7 @@
   <dimension ref="A1:V148"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A143" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A133" sqref="A114:U133"/>
+      <selection activeCell="T166" sqref="T166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>